<commit_message>
Add new ingredient densities
</commit_message>
<xml_diff>
--- a/ingredient_densities.xlsx
+++ b/ingredient_densities.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2">
   <fileVersion appName="Calc"/>
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="68">
   <si>
     <t xml:space="preserve">Ingredient</t>
   </si>
@@ -217,6 +217,15 @@
   </si>
   <si>
     <t xml:space="preserve">https://bartenderly.com/tips-tricks/alcohol-density-chart</t>
+  </si>
+  <si>
+    <t xml:space="preserve">buttermilk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">259 g/cup</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.aqua-calc.com/page/density-table/substance/milk-coma-and-blank-buttermilk-coma-and-blank-fluid-coma-and-blank-cultured-coma-and-blank-lowfat</t>
   </si>
 </sst>
 </file>
@@ -447,10 +456,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B25" activeCellId="0" sqref="B25"/>
+      <selection pane="bottomLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4609375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.4609375" defaultRowHeight="12.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="35.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="17.13"/>
@@ -856,7 +865,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
         <v>35</v>
       </c>
@@ -878,7 +887,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
         <v>40</v>
       </c>
@@ -911,7 +920,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
         <v>47</v>
       </c>
@@ -969,7 +978,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
         <v>62</v>
       </c>
@@ -978,6 +987,17 @@
       </c>
       <c r="C24" s="1" t="s">
         <v>64</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -987,6 +1007,7 @@
     <hyperlink ref="C16" r:id="rId2" display="https://www.aqua-calc.com/page/density-table/substance/corn-blank-syrup-coma-and-blank-light-blank-or-blank-dark"/>
     <hyperlink ref="C19" r:id="rId3" display="https://www.aqua-calc.com/page/density-table/substance/Cream-coma-and-blank-fluid-coma-and-blank-heavy-blank-whipping"/>
     <hyperlink ref="C24" r:id="rId4" display="https://bartenderly.com/tips-tricks/alcohol-density-chart"/>
+    <hyperlink ref="C25" r:id="rId5" display="https://www.aqua-calc.com/page/density-table/substance/milk-coma-and-blank-buttermilk-coma-and-blank-fluid-coma-and-blank-cultured-coma-and-blank-lowfat"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="1" right="1" top="1.66666666666667" bottom="1.66666666666667" header="1" footer="1"/>
@@ -1009,7 +1030,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4609375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.4609375" defaultRowHeight="12.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="1" style="1" width="10.45"/>
   </cols>
@@ -1035,7 +1056,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4609375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.4609375" defaultRowHeight="12.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="1" style="1" width="10.45"/>
   </cols>

</xml_diff>